<commit_message>
chore: atualiza arquivo da planilha
</commit_message>
<xml_diff>
--- a/T2/Planilha de gastos T2 Microcontroladores.xlsx
+++ b/T2/Planilha de gastos T2 Microcontroladores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{137238C7-1DAE-4405-8DF5-CB8EB70C250C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C9CD46-EA67-4523-B579-75077AB265FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{45FBBF5D-F628-4A8A-ABD8-EF5CCD7F7E05}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>TABELA DE PREÇOS</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Custo Total</t>
+  </si>
+  <si>
+    <t>Display touch Raspberry Pi 720 x 1280</t>
   </si>
 </sst>
 </file>
@@ -205,14 +208,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -225,6 +225,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -562,79 +571,87 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C9E371-52B4-4CB1-BBEA-2866A2F2295B}">
-  <dimension ref="C5:D12"/>
+  <dimension ref="C5:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="34.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="8"/>
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>2.1800000000000002</v>
       </c>
     </row>
     <row r="8" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="10">
+        <v>759.05</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D9" s="5">
         <v>585</v>
       </c>
     </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C9" s="5" t="s">
+    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D10" s="5">
         <v>7.5</v>
       </c>
     </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C10" s="5" t="s">
+    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D11" s="5">
         <v>4.59</v>
       </c>
     </row>
-    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C11" s="5" t="s">
+    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D12" s="5">
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C12" s="7" t="s">
+    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="8">
-        <f>ROUND(SUM(D7:D11),5)</f>
-        <v>680.27</v>
+      <c r="D13" s="7">
+        <f>ROUND(SUM(D7:D12),5)</f>
+        <v>1439.32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>